<commit_message>
APACHE POI - excel read
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/cybertek22-cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608F4A71-3EC6-F14D-A7DE-43E69930AA6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E3649D-3802-F944-85EA-B727A4F3CC75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8860" yWindow="1880" windowWidth="28040" windowHeight="17440" xr2:uid="{04502BC3-B20B-7649-90D4-6453B3FE1CF3}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
APACHE POI - excel write
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/cybertek22-cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFA4EA7-D28D-AC49-95B0-624DAE0C14EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16225A07-D2D3-B94E-8D00-3AA95A35F961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="1880" windowWidth="28040" windowHeight="17440" xr2:uid="{04502BC3-B20B-7649-90D4-6453B3FE1CF3}"/>
+    <workbookView xWindow="8960" yWindow="2300" windowWidth="28040" windowHeight="17440" xr2:uid="{04502BC3-B20B-7649-90D4-6453B3FE1CF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B89D9F-CADA-5F41-9ECC-CF10D71B94A5}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>